<commit_message>
really commit from arikan-dell 6/23-2
</commit_message>
<xml_diff>
--- a/FAQ.xlsx
+++ b/FAQ.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>编号</t>
   </si>
@@ -35,9 +35,6 @@
     <t>来源</t>
   </si>
   <si>
-    <t>日期</t>
-  </si>
-  <si>
     <t>问题</t>
   </si>
   <si>
@@ -50,13 +47,13 @@
     <t>afterpay支持几期分期？</t>
   </si>
   <si>
-    <t xml:space="preserve"> 您好，对于AfterPay的分期，我们只负责功能支持，至于具体的分期策略完全是由AfterPay决定的。通常来说Afterpay支持4期免息，这是也是最常用的分期策略。</t>
+    <t>您好，对于AfterPay的分期，我们只负责功能支持，至于具体的分期策略完全是由AfterPay决定的。通常来说Afterpay支持4期免息，这是也是最常用的分期策略。</t>
   </si>
   <si>
     <t>Google pay和Apple pay是否也支持加拿大，英国，欧洲地区？</t>
   </si>
   <si>
-    <t>我们支持的地区是和GooglePay以及ApplePay官方保持一致的，通常来说除了少部分受制裁地区，大部分国家和地区都支持。具体可参看以下官方文档https://support.google.com/pay/answer/9023773?hl=zh-Hans#zippy=%2C%E5%9C%A8%E7%BA%BF%E4%BB%98%E6%AC%BE%E6%88%96%E5%9C%A8%E5%BA%94%E7%94%A8%E5%86%85%E4%BB%98%E6%AC%BE</t>
+    <t>您好，我们支持的地区是和GooglePay以及ApplePay官方保持一致的，通常来说除了少部分受制裁地区，大部分国家和地区都支持。具体可参看以下官方文档https://support.google.com/pay/answer/9023773?hl=zh-Hans#zippy=%2C%E5%9C%A8%E7%BA%BF%E4%BB%98%E6%AC%BE%E6%88%96%E5%9C%A8%E5%BA%94%E7%94%A8%E5%86%85%E4%BB%98%E6%AC%BE</t>
   </si>
   <si>
     <t>香港深辉扬SENHUIYANG</t>
@@ -65,7 +62,64 @@
     <t>mc后台配置中心，域名管理中的域名末尾带斜杠有影响吗</t>
   </si>
   <si>
-    <t>不建议带斜杠，如果这个地方带了斜杠，其他所有使用到这个域名的地方都需要带上斜杠。也就是说要全部保持统一</t>
+    <t>您好，我们不建议带斜杠，及时带上斜杠并不会直接导致错误。因为此处的域名需要保持全局统一，如果此处带了斜杠，其他所有使用到这个域名的地方都需要带上斜杠。</t>
+  </si>
+  <si>
+    <t>BAIERTE TRADING</t>
+  </si>
+  <si>
+    <t>当发生争议时，如果客户自己取消了拒付，商家还会被收取争议处理费吗？</t>
+  </si>
+  <si>
+    <t>您好，银行对于拒付，只要发生都会收拒付处理费。客户撤销拒付只会影响拒付率的计算，而不影响银行对拒付手续费的收取。</t>
+  </si>
+  <si>
+    <t>afterpay的成功率很低是怎么回事？</t>
+  </si>
+  <si>
+    <t>您好，订单量对于成功率波动有影响，当订单数据量越多，成功率越趋于平衡，此时的订单成功率才具备较高的参考价值。当订单数据量较少时，建议先积累数据量，再观察数据表现。</t>
+  </si>
+  <si>
+    <t>TIME HONOUR</t>
+  </si>
+  <si>
+    <t>系统中没有一笔成功交易，是否可以确定是使用的通道不通畅的原因导致的呢？</t>
+  </si>
+  <si>
+    <t>您好，如果通道不通畅的话，交易是无法送入的。如果系统中存在失败交易、过期交易、处理中等状态的交易，说明通道是畅通的。此时无成功交易需要考虑其他潜在的原因。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HONGXINYI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">测试卡测试时 当天支付几次之后就无法再付款，间隔一周也不行，只能加白名单。是否可以取消掉这个风控，因为可能后续用户会有多次付费的情况。  </t>
+  </si>
+  <si>
+    <t>您好，测试卡可以通过加入白名单的形式来避免风控。实际在用户支付过程中，UseePay风控系统认为短期内多次相同金额的重复支付通常是不正常的，会触发拦截，触发条件是：24小时内，同一张卡，同一个邮箱，同一个ip，同金额订单，最多支付三次。此模式足够正常情况下的用户消费，超出3次将触发拦截。</t>
+  </si>
+  <si>
+    <t>退款是原路返回吗？这边后台能看到退款成功，但是实际卡没有收到退款。</t>
+  </si>
+  <si>
+    <t>您好，退款是3-7天内原路返回，实际处理一般很快，但并非实时到账。没有收到退款的原因通常是银行处理延迟导致。并且退款就有相对应的ARN编码生成，如消费者存在疑问可以提供ARN码以便和银行核实。 </t>
+  </si>
+  <si>
+    <t>LIGHTSPARK</t>
+  </si>
+  <si>
+    <t>为什么账户的保证金和可提现金额比例完全对不上？</t>
+  </si>
+  <si>
+    <t>您好，保证金是按照每笔交易订单的10%收取，已生成结算的订单才会开始收取保证金。所以保证金最终是占比已结算金额的10%，而不是可提现金额的10%，所以二者会有比例差异。</t>
+  </si>
+  <si>
+    <t>SENHUIYANG</t>
+  </si>
+  <si>
+    <t>支付通道是实时到账还是延时到账？</t>
+  </si>
+  <si>
+    <t>尚未回复</t>
   </si>
 </sst>
 </file>
@@ -681,15 +735,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -966,6 +1026,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -1218,20 +1285,19 @@
   <sheetPr/>
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="8.72727272727273" style="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.0909090909091" style="1" customWidth="1"/>
-    <col min="4" max="4" width="69.1818181818182" customWidth="1"/>
-    <col min="5" max="5" width="125.363636363636" customWidth="1"/>
+    <col min="3" max="3" width="70.2727272727273" style="2" customWidth="1"/>
+    <col min="4" max="4" width="125.363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1244,94 +1310,145 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45805.6513888889</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45805.6555555556</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45806.4916666667</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
commit from arikan-dell 0626 19:06
</commit_message>
<xml_diff>
--- a/FAQ.xlsx
+++ b/FAQ.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>编号</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>尚未回复</t>
+  </si>
+  <si>
+    <t>Klarna四期免息，有没有金额限制？</t>
+  </si>
+  <si>
+    <t>您好，这个根据不同的消费者信用而定，每期的免息金额一般是2500美金左右。</t>
   </si>
 </sst>
 </file>
@@ -1451,9 +1457,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1">

</xml_diff>

<commit_message>
commint from arikan-dell 0627 18:01
</commit_message>
<xml_diff>
--- a/FAQ.xlsx
+++ b/FAQ.xlsx
@@ -27,11 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>编号</t>
   </si>
   <si>
+    <t>业务</t>
+  </si>
+  <si>
     <t>来源</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
     <t>解答</t>
   </si>
   <si>
+    <t>收单</t>
+  </si>
+  <si>
     <t xml:space="preserve"> TIME HONOUR</t>
   </si>
   <si>
@@ -126,6 +132,24 @@
   </si>
   <si>
     <t>您好，这个根据不同的消费者信用而定，每期的免息金额一般是2500美金左右。</t>
+  </si>
+  <si>
+    <t>订阅</t>
+  </si>
+  <si>
+    <t>KeLing Technology Limited</t>
+  </si>
+  <si>
+    <t>订阅时对续订的扣费是UseePay自动发起的吗？</t>
+  </si>
+  <si>
+    <t>您好，订阅的续订需要商户主动调用接口进行扣费，续订时不需要消费者参与支付验证，您可通过定时任务来实现续订扣费。</t>
+  </si>
+  <si>
+    <t>为什么续订时UseePay不能自动对用户扣费？</t>
+  </si>
+  <si>
+    <t>您好，出于合规要求，UseePay不能跳过商户直接对商户的客户进行扣款，对商户用户的扣款只能由商户来发起</t>
   </si>
 </sst>
 </file>
@@ -749,13 +773,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1289,21 +1313,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="8.72727272727273" style="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.2727272727273" style="2" customWidth="1"/>
-    <col min="4" max="4" width="125.363636363636" customWidth="1"/>
+    <col min="1" max="2" width="8.72727272727273" style="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.2727272727273" style="2" customWidth="1"/>
+    <col min="5" max="5" width="125.363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1313,169 +1337,229 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:1">

</xml_diff>